<commit_message>
Changed viscosity to fix felix bug, added in low TQFM
</commit_message>
<xml_diff>
--- a/docs/Examples/Error_propagation/Cpx_Liq_Error_prop_Feig2010_example.xlsx
+++ b/docs/Examples/Error_propagation/Cpx_Liq_Error_prop_Feig2010_example.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\penny\OneDrive - Oregon State University\Postdoc\PyMME\MyBarometers\Thermobar_outer\Examples\Error_propagation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Postdoc\PyMME\MyBarometers\Thermobar_outer\docs\Examples\Error_propagation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7F6D9E5-E377-4410-8959-CE50E59F3D5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8507B948-E735-4670-BF61-B949D6D76103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{EB6A5B17-6B7D-45D9-8D27-4A36EDEB9306}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" xr2:uid="{EB6A5B17-6B7D-45D9-8D27-4A36EDEB9306}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -72,9 +72,6 @@
     <t>H2O_Liq</t>
   </si>
   <si>
-    <t>Fe3FeT_Liq</t>
-  </si>
-  <si>
     <t>NiO_Liq</t>
   </si>
   <si>
@@ -132,9 +129,6 @@
     <t>H2O_Liq_Err</t>
   </si>
   <si>
-    <t>Fe3FeT_Liq_Err</t>
-  </si>
-  <si>
     <t>NiO_Liq_Err</t>
   </si>
   <si>
@@ -208,6 +202,12 @@
   </si>
   <si>
     <t>Cr2O3_Cpx_Err</t>
+  </si>
+  <si>
+    <t>Fe3Fet_Liq</t>
+  </si>
+  <si>
+    <t>Fe3Fet_Liq_Err</t>
   </si>
 </sst>
 </file>
@@ -581,18 +581,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A138EBCD-93CC-48C3-A3EA-F033A63F0721}">
   <dimension ref="A1:BI8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AP1" workbookViewId="0">
-      <selection activeCell="BA1" sqref="BA1"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="AF2" sqref="AF2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="19" width="8.88671875" style="1"/>
+    <col min="2" max="19" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -631,153 +631,153 @@
         <v>11</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="T1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AG1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AK1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AL1" t="s">
         <v>36</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AM1" t="s">
         <v>37</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AN1" t="s">
         <v>38</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AO1" t="s">
         <v>39</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AP1" t="s">
         <v>40</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AQ1" t="s">
         <v>41</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AR1" t="s">
         <v>42</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AS1" t="s">
         <v>43</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AT1" t="s">
         <v>44</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AU1" t="s">
         <v>45</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AV1" t="s">
+        <v>15</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AX1" t="s">
         <v>46</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AY1" t="s">
         <v>47</v>
       </c>
-      <c r="AV1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AW1" t="s">
-        <v>17</v>
-      </c>
-      <c r="AX1" t="s">
+      <c r="AZ1" t="s">
         <v>48</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="BA1" t="s">
         <v>49</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BB1" t="s">
         <v>50</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BC1" t="s">
         <v>51</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BD1" t="s">
         <v>52</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BE1" t="s">
         <v>53</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BF1" t="s">
         <v>54</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BG1" t="s">
         <v>55</v>
       </c>
-      <c r="BF1" t="s">
-        <v>56</v>
-      </c>
-      <c r="BG1" t="s">
-        <v>57</v>
-      </c>
       <c r="BH1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="BI1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" s="1">
         <v>50.973845454545398</v>
@@ -960,9 +960,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="1">
         <v>53.642628571428503</v>
@@ -1145,9 +1145,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" s="1">
         <v>49.629083484573499</v>
@@ -1330,9 +1330,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1">
         <v>51.624314285714298</v>
@@ -1515,9 +1515,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" s="1">
         <v>53.980585714285702</v>
@@ -1700,9 +1700,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="1">
         <v>51.709179999999897</v>
@@ -1885,9 +1885,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="1">
         <v>53.426279999999998</v>

</xml_diff>

<commit_message>
Swapped cali datasets so loaded from csvs not pickles to solve pandas incompatability issues
</commit_message>
<xml_diff>
--- a/docs/Examples/Error_propagation/Cpx_Liq_Error_prop_Feig2010_example.xlsx
+++ b/docs/Examples/Error_propagation/Cpx_Liq_Error_prop_Feig2010_example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Postdoc\PyMME\MyBarometers\Thermobar_outer\docs\Examples\Error_propagation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/73708eac12f6644f/Documents/Postdoc_missing/MyBarometers/Thermobar_outer/docs/Examples/Error_propagation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8507B948-E735-4670-BF61-B949D6D76103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{8507B948-E735-4670-BF61-B949D6D76103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BAC5FB8C-A770-4EE7-8422-65B42CEC14D7}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" xr2:uid="{EB6A5B17-6B7D-45D9-8D27-4A36EDEB9306}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EB6A5B17-6B7D-45D9-8D27-4A36EDEB9306}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="67">
   <si>
     <t>SiO2_Liq</t>
   </si>
@@ -208,6 +208,33 @@
   </si>
   <si>
     <t>Fe3Fet_Liq_Err</t>
+  </si>
+  <si>
+    <t>Sample_ID_Liq</t>
+  </si>
+  <si>
+    <t>Feig2010_1</t>
+  </si>
+  <si>
+    <t>Feig2010_2</t>
+  </si>
+  <si>
+    <t>Feig2010_3</t>
+  </si>
+  <si>
+    <t>Feig2010_4</t>
+  </si>
+  <si>
+    <t>Feig2010_5</t>
+  </si>
+  <si>
+    <t>Feig2010_6</t>
+  </si>
+  <si>
+    <t>Feig2010_7</t>
+  </si>
+  <si>
+    <t>Sample_ID_Cpx</t>
   </si>
 </sst>
 </file>
@@ -579,233 +606,239 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A138EBCD-93CC-48C3-A3EA-F033A63F0721}">
-  <dimension ref="A1:BI8"/>
+  <dimension ref="A1:BK8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="AF2" sqref="AF2"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
+      <selection activeCell="AM2" sqref="AM2:AM8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="19" width="8.90625" style="1"/>
+    <col min="3" max="20" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
+      <c r="B1" t="s">
+        <v>58</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AK1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AN1" t="s">
         <v>36</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AO1" t="s">
         <v>37</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AP1" t="s">
         <v>38</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AQ1" t="s">
         <v>39</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AR1" t="s">
         <v>40</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AS1" t="s">
         <v>41</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AT1" t="s">
         <v>42</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AU1" t="s">
         <v>43</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AV1" t="s">
         <v>44</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AW1" t="s">
         <v>45</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AX1" t="s">
         <v>15</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AY1" t="s">
         <v>16</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AZ1" t="s">
         <v>46</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="BA1" t="s">
         <v>47</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BB1" t="s">
         <v>48</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BC1" t="s">
         <v>49</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BD1" t="s">
         <v>50</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BE1" t="s">
         <v>51</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BF1" t="s">
         <v>52</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BG1" t="s">
         <v>53</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BH1" t="s">
         <v>54</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BI1" t="s">
         <v>55</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BJ1" t="s">
         <v>34</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BK1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="1">
         <v>50.973845454545398</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D2" s="1">
         <v>0.48928181818181798</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E2" s="1">
         <v>19.349172727272698</v>
       </c>
-      <c r="E2" s="1">
+      <c r="F2" s="1">
         <v>5.32733636363636</v>
       </c>
-      <c r="F2" s="1">
-        <v>0</v>
-      </c>
       <c r="G2" s="1">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1">
         <v>4.51137272727272</v>
       </c>
-      <c r="H2" s="1">
+      <c r="I2" s="1">
         <v>9.1618727272727192</v>
       </c>
-      <c r="I2" s="1">
+      <c r="J2" s="1">
         <v>4.2055363636363596</v>
       </c>
-      <c r="J2" s="1">
-        <v>0</v>
-      </c>
       <c r="K2" s="1">
         <v>0</v>
       </c>
@@ -813,11 +846,11 @@
         <v>0</v>
       </c>
       <c r="M2" s="1">
+        <v>0</v>
+      </c>
+      <c r="N2" s="1">
         <v>5.12</v>
       </c>
-      <c r="N2" s="1">
-        <v>0</v>
-      </c>
       <c r="O2" s="1">
         <v>0</v>
       </c>
@@ -828,38 +861,38 @@
         <v>0</v>
       </c>
       <c r="R2" s="1">
+        <v>0</v>
+      </c>
+      <c r="S2" s="1">
         <v>1</v>
       </c>
-      <c r="S2" s="1">
+      <c r="T2" s="1">
         <v>1293.1500000000001</v>
       </c>
-      <c r="T2" s="2">
+      <c r="U2" s="2">
         <v>0.32603034939591202</v>
       </c>
-      <c r="U2" s="2">
+      <c r="V2" s="2">
         <v>4.24479638659334E-2</v>
       </c>
-      <c r="V2" s="2">
+      <c r="W2" s="2">
         <v>0.221883510387823</v>
       </c>
-      <c r="W2" s="2">
+      <c r="X2" s="2">
         <v>0.43268415102180002</v>
       </c>
-      <c r="X2" s="2">
-        <v>0</v>
-      </c>
       <c r="Y2" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="2">
         <v>0.20701056055627701</v>
       </c>
-      <c r="Z2" s="2">
+      <c r="AA2" s="2">
         <v>0.26804534351828302</v>
       </c>
-      <c r="AA2" s="2">
+      <c r="AB2" s="2">
         <v>0.21364690155829799</v>
       </c>
-      <c r="AB2" s="2">
-        <v>0</v>
-      </c>
       <c r="AC2" s="2">
         <v>0</v>
       </c>
@@ -867,11 +900,11 @@
         <v>0</v>
       </c>
       <c r="AE2" s="2">
+        <v>0</v>
+      </c>
+      <c r="AF2" s="2">
         <v>0.25600000000000001</v>
       </c>
-      <c r="AF2" s="2">
-        <v>0</v>
-      </c>
       <c r="AG2" s="2">
         <v>0</v>
       </c>
@@ -887,110 +920,116 @@
       <c r="AK2" s="2">
         <v>0</v>
       </c>
-      <c r="AL2">
+      <c r="AL2" s="2">
+        <v>0</v>
+      </c>
+      <c r="AM2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AN2">
         <v>51.075956440750801</v>
       </c>
-      <c r="AM2">
+      <c r="AO2">
         <v>0.32508571428571398</v>
       </c>
-      <c r="AN2">
+      <c r="AP2">
         <v>4.8925019542505597</v>
       </c>
-      <c r="AO2">
+      <c r="AQ2">
         <v>5.7149571589134203</v>
       </c>
-      <c r="AP2">
+      <c r="AR2">
         <v>0.16569999999999999</v>
       </c>
-      <c r="AQ2">
+      <c r="AS2">
         <v>16.897042208054199</v>
       </c>
-      <c r="AR2">
+      <c r="AT2">
         <v>20.466034481264099</v>
       </c>
-      <c r="AS2">
+      <c r="AU2">
         <v>0.31970395196201601</v>
       </c>
-      <c r="AT2">
-        <v>0</v>
-      </c>
-      <c r="AU2">
+      <c r="AV2">
+        <v>0</v>
+      </c>
+      <c r="AW2">
         <v>0.25218571428571401</v>
       </c>
-      <c r="AV2">
+      <c r="AX2">
         <v>1</v>
       </c>
-      <c r="AW2">
+      <c r="AY2">
         <v>1293.1500000000001</v>
       </c>
-      <c r="AX2">
+      <c r="AZ2">
         <v>0.40004424478155998</v>
       </c>
-      <c r="AY2">
+      <c r="BA2">
         <v>3.2172422381672401E-2</v>
       </c>
-      <c r="AZ2">
+      <c r="BB2">
         <v>0.51046015142187595</v>
       </c>
-      <c r="BA2">
+      <c r="BC2">
         <v>0.35767966055515299</v>
       </c>
-      <c r="BB2">
+      <c r="BD2">
         <v>2.3249014316023602E-2</v>
       </c>
-      <c r="BC2">
+      <c r="BE2">
         <v>0.538038692011093</v>
       </c>
-      <c r="BD2">
+      <c r="BF2">
         <v>0.64516379577648297</v>
       </c>
-      <c r="BE2">
+      <c r="BG2">
         <v>4.9138455746857497E-2</v>
       </c>
-      <c r="BF2">
-        <v>0</v>
-      </c>
-      <c r="BG2">
+      <c r="BH2">
+        <v>0</v>
+      </c>
+      <c r="BI2">
         <v>3.4645895792114897E-2</v>
       </c>
-      <c r="BH2">
-        <v>0</v>
-      </c>
-      <c r="BI2">
+      <c r="BJ2">
+        <v>0</v>
+      </c>
+      <c r="BK2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="1">
         <v>53.642628571428503</v>
       </c>
-      <c r="C3" s="1">
+      <c r="D3" s="1">
         <v>0.61737142857142802</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E3" s="1">
         <v>19.320971428571401</v>
       </c>
-      <c r="E3" s="1">
+      <c r="F3" s="1">
         <v>4.88498571428571</v>
       </c>
-      <c r="F3" s="1">
-        <v>0</v>
-      </c>
       <c r="G3" s="1">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1">
         <v>3.25734285714285</v>
       </c>
-      <c r="H3" s="1">
+      <c r="I3" s="1">
         <v>6.82431428571428</v>
       </c>
-      <c r="I3" s="1">
+      <c r="J3" s="1">
         <v>5.0570428571428501</v>
       </c>
-      <c r="J3" s="1">
-        <v>0</v>
-      </c>
       <c r="K3" s="1">
         <v>0</v>
       </c>
@@ -998,11 +1037,11 @@
         <v>0</v>
       </c>
       <c r="M3" s="1">
+        <v>0</v>
+      </c>
+      <c r="N3" s="1">
         <v>5.18</v>
       </c>
-      <c r="N3" s="1">
-        <v>0</v>
-      </c>
       <c r="O3" s="1">
         <v>0</v>
       </c>
@@ -1013,38 +1052,38 @@
         <v>0</v>
       </c>
       <c r="R3" s="1">
+        <v>0</v>
+      </c>
+      <c r="S3" s="1">
         <v>1.0229999999999999</v>
       </c>
-      <c r="S3" s="1">
+      <c r="T3" s="1">
         <v>1253.1500000000001</v>
       </c>
-      <c r="T3" s="2">
+      <c r="U3" s="2">
         <v>0.32869766105257597</v>
       </c>
-      <c r="U3" s="2">
+      <c r="V3" s="2">
         <v>2.5181588134039899E-2</v>
       </c>
-      <c r="V3" s="2">
+      <c r="W3" s="2">
         <v>0.24267506886338899</v>
       </c>
-      <c r="W3" s="2">
+      <c r="X3" s="2">
         <v>0.21475482476980101</v>
       </c>
-      <c r="X3" s="2">
-        <v>0</v>
-      </c>
       <c r="Y3" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="2">
         <v>0.16329163947921099</v>
       </c>
-      <c r="Z3" s="2">
+      <c r="AA3" s="2">
         <v>0.17171743678276</v>
       </c>
-      <c r="AA3" s="2">
+      <c r="AB3" s="2">
         <v>8.5388345362879994E-2</v>
       </c>
-      <c r="AB3" s="2">
-        <v>0</v>
-      </c>
       <c r="AC3" s="2">
         <v>0</v>
       </c>
@@ -1052,11 +1091,11 @@
         <v>0</v>
       </c>
       <c r="AE3" s="2">
+        <v>0</v>
+      </c>
+      <c r="AF3" s="2">
         <v>0.25900000000000001</v>
       </c>
-      <c r="AF3" s="2">
-        <v>0</v>
-      </c>
       <c r="AG3" s="2">
         <v>0</v>
       </c>
@@ -1072,110 +1111,116 @@
       <c r="AK3" s="2">
         <v>0</v>
       </c>
-      <c r="AL3">
+      <c r="AL3" s="2">
+        <v>0</v>
+      </c>
+      <c r="AM3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AN3">
         <v>51.57835</v>
       </c>
-      <c r="AM3">
+      <c r="AO3">
         <v>0.35685999999999901</v>
       </c>
-      <c r="AN3">
+      <c r="AP3">
         <v>3.6001999999999899</v>
       </c>
-      <c r="AO3">
+      <c r="AQ3">
         <v>6.39018</v>
       </c>
-      <c r="AP3">
+      <c r="AR3">
         <v>0.17119000000000001</v>
       </c>
-      <c r="AQ3">
+      <c r="AS3">
         <v>16.402000000000001</v>
       </c>
-      <c r="AR3">
+      <c r="AT3">
         <v>20.388059999999999</v>
       </c>
-      <c r="AS3">
+      <c r="AU3">
         <v>0.33272000000000002</v>
       </c>
-      <c r="AT3">
-        <v>0</v>
-      </c>
-      <c r="AU3">
+      <c r="AV3">
+        <v>0</v>
+      </c>
+      <c r="AW3">
         <v>0.18626999999999999</v>
       </c>
-      <c r="AV3">
+      <c r="AX3">
         <v>1.0229999999999999</v>
       </c>
-      <c r="AW3">
+      <c r="AY3">
         <v>1253.1500000000001</v>
       </c>
-      <c r="AX3">
+      <c r="AZ3">
         <v>0.62806409837438903</v>
       </c>
-      <c r="AY3">
+      <c r="BA3">
         <v>6.7227312571272402E-2</v>
       </c>
-      <c r="AZ3">
+      <c r="BB3">
         <v>0.62260115465503196</v>
       </c>
-      <c r="BA3">
+      <c r="BC3">
         <v>0.65747624680371597</v>
       </c>
-      <c r="BB3">
+      <c r="BD3">
         <v>5.0037107341563102E-2</v>
       </c>
-      <c r="BC3">
+      <c r="BE3">
         <v>0.73281638142776195</v>
       </c>
-      <c r="BD3">
+      <c r="BF3">
         <v>1.0507576802795899</v>
       </c>
-      <c r="BE3">
+      <c r="BG3">
         <v>6.0947678836486802E-2</v>
       </c>
-      <c r="BF3">
-        <v>0</v>
-      </c>
-      <c r="BG3">
+      <c r="BH3">
+        <v>0</v>
+      </c>
+      <c r="BI3">
         <v>6.20947671797802E-2</v>
       </c>
-      <c r="BH3">
-        <v>0</v>
-      </c>
-      <c r="BI3">
+      <c r="BJ3">
+        <v>0</v>
+      </c>
+      <c r="BK3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="1">
         <v>49.629083484573499</v>
       </c>
-      <c r="C4" s="1">
+      <c r="D4" s="1">
         <v>0.36578749999999999</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E4" s="1">
         <v>19.103074652812801</v>
       </c>
-      <c r="E4" s="1">
+      <c r="F4" s="1">
         <v>5.3028600587194301</v>
       </c>
-      <c r="F4" s="1">
-        <v>0</v>
-      </c>
       <c r="G4" s="1">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1">
         <v>6.4033765103420004</v>
       </c>
-      <c r="H4" s="1">
+      <c r="I4" s="1">
         <v>11.6159427643596</v>
       </c>
-      <c r="I4" s="1">
+      <c r="J4" s="1">
         <v>3.27578298879153</v>
       </c>
-      <c r="J4" s="1">
-        <v>0</v>
-      </c>
       <c r="K4" s="1">
         <v>0</v>
       </c>
@@ -1183,11 +1228,11 @@
         <v>0</v>
       </c>
       <c r="M4" s="1">
+        <v>0</v>
+      </c>
+      <c r="N4" s="1">
         <v>5.05</v>
       </c>
-      <c r="N4" s="1">
-        <v>0</v>
-      </c>
       <c r="O4" s="1">
         <v>0</v>
       </c>
@@ -1198,38 +1243,38 @@
         <v>0</v>
       </c>
       <c r="R4" s="1">
+        <v>0</v>
+      </c>
+      <c r="S4" s="1">
         <v>1.0169999999999999</v>
       </c>
-      <c r="S4" s="1">
+      <c r="T4" s="1">
         <v>1333.15</v>
       </c>
-      <c r="T4" s="2">
+      <c r="U4" s="2">
         <v>0.476010705190619</v>
       </c>
-      <c r="U4" s="2">
+      <c r="V4" s="2">
         <v>2.70828589702043E-2</v>
       </c>
-      <c r="V4" s="2">
+      <c r="W4" s="2">
         <v>0.23581414640857601</v>
       </c>
-      <c r="W4" s="2">
+      <c r="X4" s="2">
         <v>0.30169564047995501</v>
       </c>
-      <c r="X4" s="2">
-        <v>0</v>
-      </c>
       <c r="Y4" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="2">
         <v>0.17443639081606899</v>
       </c>
-      <c r="Z4" s="2">
+      <c r="AA4" s="2">
         <v>0.206030250148626</v>
       </c>
-      <c r="AA4" s="2">
+      <c r="AB4" s="2">
         <v>0.22958289062002499</v>
       </c>
-      <c r="AB4" s="2">
-        <v>0</v>
-      </c>
       <c r="AC4" s="2">
         <v>0</v>
       </c>
@@ -1237,11 +1282,11 @@
         <v>0</v>
       </c>
       <c r="AE4" s="2">
+        <v>0</v>
+      </c>
+      <c r="AF4" s="2">
         <v>0.2525</v>
       </c>
-      <c r="AF4" s="2">
-        <v>0</v>
-      </c>
       <c r="AG4" s="2">
         <v>0</v>
       </c>
@@ -1257,110 +1302,116 @@
       <c r="AK4" s="2">
         <v>0</v>
       </c>
-      <c r="AL4">
+      <c r="AL4" s="2">
+        <v>0</v>
+      </c>
+      <c r="AM4" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AN4">
         <v>51.5678750537326</v>
       </c>
-      <c r="AM4">
+      <c r="AO4">
         <v>0.25627142857142798</v>
       </c>
-      <c r="AN4">
+      <c r="AP4">
         <v>4.7638067089279303</v>
       </c>
-      <c r="AO4">
+      <c r="AQ4">
         <v>4.2290210045395398</v>
       </c>
-      <c r="AP4">
-        <v>0</v>
-      </c>
-      <c r="AQ4">
+      <c r="AR4">
+        <v>0</v>
+      </c>
+      <c r="AS4">
         <v>16.9693441092036</v>
       </c>
-      <c r="AR4">
+      <c r="AT4">
         <v>21.061352033077</v>
       </c>
-      <c r="AS4">
+      <c r="AU4">
         <v>0.31650607457058999</v>
       </c>
-      <c r="AT4">
-        <v>0</v>
-      </c>
-      <c r="AU4">
+      <c r="AV4">
+        <v>0</v>
+      </c>
+      <c r="AW4">
         <v>0.52892857142857097</v>
       </c>
-      <c r="AV4">
+      <c r="AX4">
         <v>1.0169999999999999</v>
       </c>
-      <c r="AW4">
+      <c r="AY4">
         <v>1333.15</v>
       </c>
-      <c r="AX4">
+      <c r="AZ4">
         <v>0.58559561653451897</v>
       </c>
-      <c r="AY4">
+      <c r="BA4">
         <v>3.2846446499112503E-2</v>
       </c>
-      <c r="AZ4">
+      <c r="BB4">
         <v>0.91876838570477404</v>
       </c>
-      <c r="BA4">
+      <c r="BC4">
         <v>0.50639171883246803</v>
       </c>
-      <c r="BB4">
-        <v>0</v>
-      </c>
-      <c r="BC4">
+      <c r="BD4">
+        <v>0</v>
+      </c>
+      <c r="BE4">
         <v>0.56226616303482102</v>
       </c>
-      <c r="BD4">
+      <c r="BF4">
         <v>0.79430966903702505</v>
       </c>
-      <c r="BE4">
+      <c r="BG4">
         <v>0.10709490569695</v>
       </c>
-      <c r="BF4">
-        <v>0</v>
-      </c>
-      <c r="BG4">
+      <c r="BH4">
+        <v>0</v>
+      </c>
+      <c r="BI4">
         <v>0.21011411751938999</v>
       </c>
-      <c r="BH4">
-        <v>0</v>
-      </c>
-      <c r="BI4">
+      <c r="BJ4">
+        <v>0</v>
+      </c>
+      <c r="BK4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="1">
         <v>51.624314285714298</v>
       </c>
-      <c r="C5" s="1">
+      <c r="D5" s="1">
         <v>0.44387142857142797</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E5" s="1">
         <v>18.451099999999901</v>
       </c>
-      <c r="E5" s="1">
+      <c r="F5" s="1">
         <v>6.3030714285714202</v>
       </c>
-      <c r="F5" s="1">
-        <v>0</v>
-      </c>
       <c r="G5" s="1">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1">
         <v>6.1322285714285698</v>
       </c>
-      <c r="H5" s="1">
+      <c r="I5" s="1">
         <v>10.365057142857101</v>
       </c>
-      <c r="I5" s="1">
+      <c r="J5" s="1">
         <v>3.6857142857142802</v>
       </c>
-      <c r="J5" s="1">
-        <v>0</v>
-      </c>
       <c r="K5" s="1">
         <v>0</v>
       </c>
@@ -1368,11 +1419,11 @@
         <v>0</v>
       </c>
       <c r="M5" s="1">
+        <v>0</v>
+      </c>
+      <c r="N5" s="1">
         <v>2.67</v>
       </c>
-      <c r="N5" s="1">
-        <v>0</v>
-      </c>
       <c r="O5" s="1">
         <v>0</v>
       </c>
@@ -1383,38 +1434,38 @@
         <v>0</v>
       </c>
       <c r="R5" s="1">
+        <v>0</v>
+      </c>
+      <c r="S5" s="1">
         <v>0.99450000000000005</v>
       </c>
-      <c r="S5" s="1">
+      <c r="T5" s="1">
         <v>1373.15</v>
       </c>
-      <c r="T5" s="2">
+      <c r="U5" s="2">
         <v>0.44289410483031599</v>
       </c>
-      <c r="U5" s="2">
+      <c r="V5" s="2">
         <v>4.7517425375179403E-2</v>
       </c>
-      <c r="V5" s="2">
+      <c r="W5" s="2">
         <v>0.23480828349979899</v>
       </c>
-      <c r="W5" s="2">
+      <c r="X5" s="2">
         <v>0.21978000905666301</v>
       </c>
-      <c r="X5" s="2">
-        <v>0</v>
-      </c>
       <c r="Y5" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="2">
         <v>0.17179946366125201</v>
       </c>
-      <c r="Z5" s="2">
+      <c r="AA5" s="2">
         <v>0.27448421847253801</v>
       </c>
-      <c r="AA5" s="2">
+      <c r="AB5" s="2">
         <v>0.25975734464157502</v>
       </c>
-      <c r="AB5" s="2">
-        <v>0</v>
-      </c>
       <c r="AC5" s="2">
         <v>0</v>
       </c>
@@ -1422,11 +1473,11 @@
         <v>0</v>
       </c>
       <c r="AE5" s="2">
+        <v>0</v>
+      </c>
+      <c r="AF5" s="2">
         <v>0.13350000000000001</v>
       </c>
-      <c r="AF5" s="2">
-        <v>0</v>
-      </c>
       <c r="AG5" s="2">
         <v>0</v>
       </c>
@@ -1442,110 +1493,116 @@
       <c r="AK5" s="2">
         <v>0</v>
       </c>
-      <c r="AL5">
+      <c r="AL5" s="2">
+        <v>0</v>
+      </c>
+      <c r="AM5" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AN5">
         <v>52.083949999999902</v>
       </c>
-      <c r="AM5">
+      <c r="AO5">
         <v>0.32598333333333301</v>
       </c>
-      <c r="AN5">
+      <c r="AP5">
         <v>3.9195666666666602</v>
       </c>
-      <c r="AO5">
+      <c r="AQ5">
         <v>5.2853166666666596</v>
       </c>
-      <c r="AP5">
+      <c r="AR5">
         <v>0.168583333333333</v>
       </c>
-      <c r="AQ5">
+      <c r="AS5">
         <v>16.604683333333298</v>
       </c>
-      <c r="AR5">
+      <c r="AT5">
         <v>20.364049999999999</v>
       </c>
-      <c r="AS5">
+      <c r="AU5">
         <v>0.318066666666666</v>
       </c>
-      <c r="AT5">
-        <v>0</v>
-      </c>
-      <c r="AU5">
+      <c r="AV5">
+        <v>0</v>
+      </c>
+      <c r="AW5">
         <v>0.377936554227017</v>
       </c>
-      <c r="AV5">
+      <c r="AX5">
         <v>0.99450000000000005</v>
       </c>
-      <c r="AW5">
+      <c r="AY5">
         <v>1373.15</v>
       </c>
-      <c r="AX5">
+      <c r="AZ5">
         <v>0.16527715813391</v>
       </c>
-      <c r="AY5">
+      <c r="BA5">
         <v>3.2708678766753499E-2</v>
       </c>
-      <c r="AZ5">
+      <c r="BB5">
         <v>0.24092356187526301</v>
       </c>
-      <c r="BA5">
+      <c r="BC5">
         <v>0.207265601744866</v>
       </c>
-      <c r="BB5">
+      <c r="BD5">
         <v>5.1433740547102501E-2</v>
       </c>
-      <c r="BC5">
+      <c r="BE5">
         <v>0.182666038623786</v>
       </c>
-      <c r="BD5">
+      <c r="BF5">
         <v>0.35548708415361002</v>
       </c>
-      <c r="BE5">
+      <c r="BG5">
         <v>4.8978838968136797E-2</v>
       </c>
-      <c r="BF5">
-        <v>0</v>
-      </c>
-      <c r="BG5">
+      <c r="BH5">
+        <v>0</v>
+      </c>
+      <c r="BI5">
         <v>5.8814436104113903E-2</v>
       </c>
-      <c r="BH5">
-        <v>0</v>
-      </c>
-      <c r="BI5">
+      <c r="BJ5">
+        <v>0</v>
+      </c>
+      <c r="BK5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="1">
         <v>53.980585714285702</v>
       </c>
-      <c r="C6" s="1">
+      <c r="D6" s="1">
         <v>0.81747142857142796</v>
       </c>
-      <c r="D6" s="1">
+      <c r="E6" s="1">
         <v>17.454985714285701</v>
       </c>
-      <c r="E6" s="1">
+      <c r="F6" s="1">
         <v>6.7444285714285703</v>
       </c>
-      <c r="F6" s="1">
-        <v>0</v>
-      </c>
       <c r="G6" s="1">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1">
         <v>5.1490999999999998</v>
       </c>
-      <c r="H6" s="1">
+      <c r="I6" s="1">
         <v>9.0308714285714196</v>
       </c>
-      <c r="I6" s="1">
+      <c r="J6" s="1">
         <v>4.1795428571428497</v>
       </c>
-      <c r="J6" s="1">
-        <v>0</v>
-      </c>
       <c r="K6" s="1">
         <v>0</v>
       </c>
@@ -1553,11 +1610,11 @@
         <v>0</v>
       </c>
       <c r="M6" s="1">
+        <v>0</v>
+      </c>
+      <c r="N6" s="1">
         <v>2.25</v>
       </c>
-      <c r="N6" s="1">
-        <v>0</v>
-      </c>
       <c r="O6" s="1">
         <v>0</v>
       </c>
@@ -1568,38 +1625,38 @@
         <v>0</v>
       </c>
       <c r="R6" s="1">
+        <v>0</v>
+      </c>
+      <c r="S6" s="1">
         <v>0.99450000000000005</v>
       </c>
-      <c r="S6" s="1">
+      <c r="T6" s="1">
         <v>1373.15</v>
       </c>
-      <c r="T6" s="2">
+      <c r="U6" s="2">
         <v>0.44535645434801702</v>
       </c>
-      <c r="U6" s="2">
+      <c r="V6" s="2">
         <v>4.39631555693989E-2</v>
       </c>
-      <c r="V6" s="2">
+      <c r="W6" s="2">
         <v>0.316155317465803</v>
       </c>
-      <c r="W6" s="2">
+      <c r="X6" s="2">
         <v>0.38931132235563098</v>
       </c>
-      <c r="X6" s="2">
-        <v>0</v>
-      </c>
       <c r="Y6" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="2">
         <v>0.13465889003946999</v>
       </c>
-      <c r="Z6" s="2">
+      <c r="AA6" s="2">
         <v>0.20904456234893101</v>
       </c>
-      <c r="AA6" s="2">
+      <c r="AB6" s="2">
         <v>0.45372268644015301</v>
       </c>
-      <c r="AB6" s="2">
-        <v>0</v>
-      </c>
       <c r="AC6" s="2">
         <v>0</v>
       </c>
@@ -1607,11 +1664,11 @@
         <v>0</v>
       </c>
       <c r="AE6" s="2">
+        <v>0</v>
+      </c>
+      <c r="AF6" s="2">
         <v>0.1125</v>
       </c>
-      <c r="AF6" s="2">
-        <v>0</v>
-      </c>
       <c r="AG6" s="2">
         <v>0</v>
       </c>
@@ -1627,110 +1684,116 @@
       <c r="AK6" s="2">
         <v>0</v>
       </c>
-      <c r="AL6">
+      <c r="AL6" s="2">
+        <v>0</v>
+      </c>
+      <c r="AM6" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AN6">
         <v>52.331846138334299</v>
       </c>
-      <c r="AM6">
+      <c r="AO6">
         <v>0.40617500000000001</v>
       </c>
-      <c r="AN6">
+      <c r="AP6">
         <v>3.9746103620449098</v>
       </c>
-      <c r="AO6">
+      <c r="AQ6">
         <v>6.0399070945945903</v>
       </c>
-      <c r="AP6">
+      <c r="AR6">
         <v>0.173175</v>
       </c>
-      <c r="AQ6">
+      <c r="AS6">
         <v>16.297102191275801</v>
       </c>
-      <c r="AR6">
+      <c r="AT6">
         <v>19.784782829307801</v>
       </c>
-      <c r="AS6">
+      <c r="AU6">
         <v>0.38886271128666799</v>
       </c>
-      <c r="AT6">
-        <v>0</v>
-      </c>
-      <c r="AU6">
+      <c r="AV6">
+        <v>0</v>
+      </c>
+      <c r="AW6">
         <v>0.28597499999999998</v>
       </c>
-      <c r="AV6">
+      <c r="AX6">
         <v>0.99450000000000005</v>
       </c>
-      <c r="AW6">
+      <c r="AY6">
         <v>1373.15</v>
       </c>
-      <c r="AX6">
+      <c r="AZ6">
         <v>0.10650879467775901</v>
       </c>
-      <c r="AY6">
+      <c r="BA6">
         <v>4.0535118518802003E-2</v>
       </c>
-      <c r="AZ6">
+      <c r="BB6">
         <v>0.47996201242306902</v>
       </c>
-      <c r="BA6">
+      <c r="BC6">
         <v>0.42888561596033897</v>
       </c>
-      <c r="BB6">
+      <c r="BD6">
         <v>2.6672879484599898E-2</v>
       </c>
-      <c r="BC6">
+      <c r="BE6">
         <v>0.43154976831285102</v>
       </c>
-      <c r="BD6">
+      <c r="BF6">
         <v>0.48626369016024401</v>
       </c>
-      <c r="BE6">
+      <c r="BG6">
         <v>5.6668054129084898E-2</v>
       </c>
-      <c r="BF6">
-        <v>0</v>
-      </c>
-      <c r="BG6">
+      <c r="BH6">
+        <v>0</v>
+      </c>
+      <c r="BI6">
         <v>5.1372130901232202E-2</v>
       </c>
-      <c r="BH6">
-        <v>0</v>
-      </c>
-      <c r="BI6">
+      <c r="BJ6">
+        <v>0</v>
+      </c>
+      <c r="BK6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="1">
         <v>51.709179999999897</v>
       </c>
-      <c r="C7" s="1">
+      <c r="D7" s="1">
         <v>0.47595999999999999</v>
       </c>
-      <c r="D7" s="1">
+      <c r="E7" s="1">
         <v>17.754359999999998</v>
       </c>
-      <c r="E7" s="1">
+      <c r="F7" s="1">
         <v>6.4681600000000001</v>
       </c>
-      <c r="F7" s="1">
-        <v>0</v>
-      </c>
       <c r="G7" s="1">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
         <v>6.9529199999999998</v>
       </c>
-      <c r="H7" s="1">
+      <c r="I7" s="1">
         <v>11.39302</v>
       </c>
-      <c r="I7" s="1">
+      <c r="J7" s="1">
         <v>3.4430999999999998</v>
       </c>
-      <c r="J7" s="1">
-        <v>0</v>
-      </c>
       <c r="K7" s="1">
         <v>0</v>
       </c>
@@ -1738,11 +1801,11 @@
         <v>0</v>
       </c>
       <c r="M7" s="1">
+        <v>0</v>
+      </c>
+      <c r="N7" s="1">
         <v>1.28</v>
       </c>
-      <c r="N7" s="1">
-        <v>0</v>
-      </c>
       <c r="O7" s="1">
         <v>0</v>
       </c>
@@ -1753,38 +1816,38 @@
         <v>0</v>
       </c>
       <c r="R7" s="1">
+        <v>0</v>
+      </c>
+      <c r="S7" s="1">
         <v>1.0085</v>
       </c>
-      <c r="S7" s="1">
+      <c r="T7" s="1">
         <v>1413.15</v>
       </c>
-      <c r="T7" s="2">
+      <c r="U7" s="2">
         <v>0.64860123496698896</v>
       </c>
-      <c r="U7" s="2">
+      <c r="V7" s="2">
         <v>3.4294431034790601E-2</v>
       </c>
-      <c r="V7" s="2">
+      <c r="W7" s="2">
         <v>0.17209457574245199</v>
       </c>
-      <c r="W7" s="2">
+      <c r="X7" s="2">
         <v>0.18235212639286799</v>
       </c>
-      <c r="X7" s="2">
-        <v>0</v>
-      </c>
       <c r="Y7" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="2">
         <v>0.27783079742892097</v>
       </c>
-      <c r="Z7" s="2">
+      <c r="AA7" s="2">
         <v>0.193893300554839</v>
       </c>
-      <c r="AA7" s="2">
+      <c r="AB7" s="2">
         <v>0.119701441094094</v>
       </c>
-      <c r="AB7" s="2">
-        <v>0</v>
-      </c>
       <c r="AC7" s="2">
         <v>0</v>
       </c>
@@ -1792,11 +1855,11 @@
         <v>0</v>
       </c>
       <c r="AE7" s="2">
+        <v>0</v>
+      </c>
+      <c r="AF7" s="2">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="AF7" s="2">
-        <v>0</v>
-      </c>
       <c r="AG7" s="2">
         <v>0</v>
       </c>
@@ -1812,110 +1875,116 @@
       <c r="AK7" s="2">
         <v>0</v>
       </c>
-      <c r="AL7">
+      <c r="AL7" s="2">
+        <v>0</v>
+      </c>
+      <c r="AM7" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AN7">
         <v>52.214879999999901</v>
       </c>
-      <c r="AM7">
+      <c r="AO7">
         <v>0.32278000000000001</v>
       </c>
-      <c r="AN7">
+      <c r="AP7">
         <v>4.8742400000000004</v>
       </c>
-      <c r="AO7">
+      <c r="AQ7">
         <v>4.8402399999999997</v>
       </c>
-      <c r="AP7">
+      <c r="AR7">
         <v>0.13838</v>
       </c>
-      <c r="AQ7">
+      <c r="AS7">
         <v>16.199279999999899</v>
       </c>
-      <c r="AR7">
+      <c r="AT7">
         <v>19.9587</v>
       </c>
-      <c r="AS7">
+      <c r="AU7">
         <v>0.48677999999999999</v>
       </c>
-      <c r="AT7">
-        <v>0</v>
-      </c>
-      <c r="AU7">
+      <c r="AV7">
+        <v>0</v>
+      </c>
+      <c r="AW7">
         <v>0.55153999999999903</v>
       </c>
-      <c r="AV7">
+      <c r="AX7">
         <v>1.0085</v>
       </c>
-      <c r="AW7">
+      <c r="AY7">
         <v>1413.15</v>
       </c>
-      <c r="AX7">
+      <c r="AZ7">
         <v>0.184704756304299</v>
       </c>
-      <c r="AY7">
+      <c r="BA7">
         <v>5.2257602317748703E-2</v>
       </c>
-      <c r="AZ7">
+      <c r="BB7">
         <v>0.37020109805347601</v>
       </c>
-      <c r="BA7">
+      <c r="BC7">
         <v>0.382829287019683</v>
       </c>
-      <c r="BB7">
+      <c r="BD7">
         <v>4.3669405766508899E-2</v>
       </c>
-      <c r="BC7">
+      <c r="BE7">
         <v>0.37707273436303002</v>
       </c>
-      <c r="BD7">
+      <c r="BF7">
         <v>3.6974315410005697E-2</v>
       </c>
-      <c r="BE7">
+      <c r="BG7">
         <v>3.2090606102099399E-2</v>
       </c>
-      <c r="BF7">
-        <v>0</v>
-      </c>
-      <c r="BG7">
+      <c r="BH7">
+        <v>0</v>
+      </c>
+      <c r="BI7">
         <v>5.6630230442759E-2</v>
       </c>
-      <c r="BH7">
-        <v>0</v>
-      </c>
-      <c r="BI7">
+      <c r="BJ7">
+        <v>0</v>
+      </c>
+      <c r="BK7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="1">
         <v>53.426279999999998</v>
       </c>
-      <c r="C8" s="1">
+      <c r="D8" s="1">
         <v>0.50141999999999998</v>
       </c>
-      <c r="D8" s="1">
+      <c r="E8" s="1">
         <v>18.53454</v>
       </c>
-      <c r="E8" s="1">
+      <c r="F8" s="1">
         <v>4.5744600000000002</v>
       </c>
-      <c r="F8" s="1">
-        <v>0</v>
-      </c>
       <c r="G8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
         <v>7.3860599999999899</v>
       </c>
-      <c r="H8" s="1">
+      <c r="I8" s="1">
         <v>11.2819799999999</v>
       </c>
-      <c r="I8" s="1">
+      <c r="J8" s="1">
         <v>3.6730999999999998</v>
       </c>
-      <c r="J8" s="1">
-        <v>0</v>
-      </c>
       <c r="K8" s="1">
         <v>0</v>
       </c>
@@ -1923,11 +1992,11 @@
         <v>0</v>
       </c>
       <c r="M8" s="1">
+        <v>0</v>
+      </c>
+      <c r="N8" s="1">
         <v>0.98</v>
       </c>
-      <c r="N8" s="1">
-        <v>0</v>
-      </c>
       <c r="O8" s="1">
         <v>0</v>
       </c>
@@ -1938,38 +2007,38 @@
         <v>0</v>
       </c>
       <c r="R8" s="1">
+        <v>0</v>
+      </c>
+      <c r="S8" s="1">
         <v>1.0085</v>
       </c>
-      <c r="S8" s="1">
+      <c r="T8" s="1">
         <v>1413.15</v>
       </c>
-      <c r="T8" s="2">
+      <c r="U8" s="2">
         <v>0.396578840838194</v>
       </c>
-      <c r="U8" s="2">
+      <c r="V8" s="2">
         <v>4.5703851041241902E-2</v>
       </c>
-      <c r="V8" s="2">
+      <c r="W8" s="2">
         <v>0.33160185916241902</v>
       </c>
-      <c r="W8" s="2">
+      <c r="X8" s="2">
         <v>0.179875020500329</v>
       </c>
-      <c r="X8" s="2">
-        <v>0</v>
-      </c>
       <c r="Y8" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="2">
         <v>0.52116380150584396</v>
       </c>
-      <c r="Z8" s="2">
+      <c r="AA8" s="2">
         <v>0.389117427006345</v>
       </c>
-      <c r="AA8" s="2">
+      <c r="AB8" s="2">
         <v>9.23930733334489E-2</v>
       </c>
-      <c r="AB8" s="2">
-        <v>0</v>
-      </c>
       <c r="AC8" s="2">
         <v>0</v>
       </c>
@@ -1977,11 +2046,11 @@
         <v>0</v>
       </c>
       <c r="AE8" s="2">
+        <v>0</v>
+      </c>
+      <c r="AF8" s="2">
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="AF8" s="2">
-        <v>0</v>
-      </c>
       <c r="AG8" s="2">
         <v>0</v>
       </c>
@@ -1997,76 +2066,82 @@
       <c r="AK8" s="2">
         <v>0</v>
       </c>
-      <c r="AL8">
+      <c r="AL8" s="2">
+        <v>0</v>
+      </c>
+      <c r="AM8" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AN8">
         <v>52.497999999999998</v>
       </c>
-      <c r="AM8">
+      <c r="AO8">
         <v>0.29976666666666602</v>
       </c>
-      <c r="AN8">
+      <c r="AP8">
         <v>3.5178666666666598</v>
       </c>
-      <c r="AO8">
+      <c r="AQ8">
         <v>5.9030666666666596</v>
       </c>
-      <c r="AP8">
+      <c r="AR8">
         <v>0.17886666666666601</v>
       </c>
-      <c r="AQ8">
+      <c r="AS8">
         <v>17.869733333333301</v>
       </c>
-      <c r="AR8">
+      <c r="AT8">
         <v>19.342233333333301</v>
       </c>
-      <c r="AS8">
+      <c r="AU8">
         <v>0.32203333333333301</v>
       </c>
-      <c r="AT8">
-        <v>0</v>
-      </c>
-      <c r="AU8">
+      <c r="AV8">
+        <v>0</v>
+      </c>
+      <c r="AW8">
         <v>0.37769999999999998</v>
       </c>
-      <c r="AV8">
+      <c r="AX8">
         <v>1.0085</v>
       </c>
-      <c r="AW8">
+      <c r="AY8">
         <v>1413.15</v>
       </c>
-      <c r="AX8">
+      <c r="AZ8">
         <v>0.10282126239383101</v>
       </c>
-      <c r="AY8">
+      <c r="BA8">
         <v>2.27932153648105E-2</v>
       </c>
-      <c r="AZ8">
+      <c r="BB8">
         <v>0.216428174382779</v>
       </c>
-      <c r="BA8">
+      <c r="BC8">
         <v>0.39593001738524097</v>
       </c>
-      <c r="BB8">
+      <c r="BD8">
         <v>1.37278791758476E-2</v>
       </c>
-      <c r="BC8">
+      <c r="BE8">
         <v>0.14473399969140199</v>
       </c>
-      <c r="BD8">
+      <c r="BF8">
         <v>0.30338486888210198</v>
       </c>
-      <c r="BE8">
+      <c r="BG8">
         <v>2.2490412772260899E-2</v>
       </c>
-      <c r="BF8">
-        <v>0</v>
-      </c>
-      <c r="BG8">
+      <c r="BH8">
+        <v>0</v>
+      </c>
+      <c r="BI8">
         <v>5.1098180006728298E-2</v>
       </c>
-      <c r="BH8">
-        <v>0</v>
-      </c>
-      <c r="BI8">
+      <c r="BJ8">
+        <v>0</v>
+      </c>
+      <c r="BK8">
         <v>0</v>
       </c>
     </row>

</xml_diff>